<commit_message>
insert 5, 6, 7, 8 to next collumn form anotherFolder
</commit_message>
<xml_diff>
--- a/exel.xlsx
+++ b/exel.xlsx
@@ -342,32 +342,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1">
         <v>1</v>
       </c>
+      <c r="B1">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>2</v>
       </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>3</v>
       </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>4</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>